<commit_message>
added new intent fasility
</commit_message>
<xml_diff>
--- a/train.xlsx
+++ b/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChatbotPerpusBipa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E119EA8A-7C67-432E-BEA5-E999C7C37BF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94436DC3-80B2-4687-A885-0842B76A1763}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="991">
   <si>
     <t>text</t>
   </si>
@@ -2645,6 +2645,354 @@
   </si>
   <si>
     <t>Yes, iya</t>
+  </si>
+  <si>
+    <t>Ada fasilitas wifi di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Fasilitas apa saja yang tersedia?</t>
+  </si>
+  <si>
+    <t>Saya mau tahu tentang ruang diskusi.</t>
+  </si>
+  <si>
+    <t>Apakah ada ruang belajar kelompok?</t>
+  </si>
+  <si>
+    <t>Perpustakaan punya area membaca nyaman?</t>
+  </si>
+  <si>
+    <t>Apakah tersedia ruang baca pribadi?</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu apa saja fasilitas di perpustakaan.</t>
+  </si>
+  <si>
+    <t>Ada ruang untuk belajar kelompok di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Perpustakaan ada layanan internet gratis?</t>
+  </si>
+  <si>
+    <t>Bisa mengakses wifi di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Fasilitas untuk diskusi bareng ada?</t>
+  </si>
+  <si>
+    <t>Ada ruang quiet zone untuk belajar?</t>
+  </si>
+  <si>
+    <t>Apa saja fasilitas umum di perpustakaan ini?</t>
+  </si>
+  <si>
+    <t>Kalau mau cari ruang baca  ada?</t>
+  </si>
+  <si>
+    <t>Saya butuh tempat diskusi  ada?</t>
+  </si>
+  <si>
+    <t>fasilitas</t>
+  </si>
+  <si>
+    <t>Apakah tersedia layanan penelusuran literatur?</t>
+  </si>
+  <si>
+    <t>Di perpustakaan bisa bantu cari jurnal?</t>
+  </si>
+  <si>
+    <t>Ada fasilitas untuk penelusuran skripsi?</t>
+  </si>
+  <si>
+    <t>Apakah ada layanan penelusuran jurnal ilmiah?</t>
+  </si>
+  <si>
+    <t>Perpustakaan menyediakan fotokopi koleksi?</t>
+  </si>
+  <si>
+    <t>Dimana saya bisa fotokopi koleksi perpustakaan?</t>
+  </si>
+  <si>
+    <t>Ada fasilitas fotokopi dokumen?</t>
+  </si>
+  <si>
+    <t>Apakah ada ruang baca umum di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Saya mau cari ruang baca, ada?</t>
+  </si>
+  <si>
+    <t>Dimana lokasi ruang baca di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Ada ruang baca nyaman untuk mahasiswa?</t>
+  </si>
+  <si>
+    <t>Bolehkah menggunakan ruang baca di sana?</t>
+  </si>
+  <si>
+    <t>Apakah ada locker untuk tas?</t>
+  </si>
+  <si>
+    <t>Di mana tempat simpan tas dan jaket?</t>
+  </si>
+  <si>
+    <t>Bisa menitipkan barang di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Ada locker penyimpanan barang pribadi?</t>
+  </si>
+  <si>
+    <t>Locker tas tersedia di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Apakah ada akses internet gratis di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Bisa menggunakan WiFi di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Ada fasilitas internet untuk pengunjung?</t>
+  </si>
+  <si>
+    <t>Bagaimana cara akses WiFi di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Internet tersedia di area perpustakaan?</t>
+  </si>
+  <si>
+    <t>Fasilitas apa saja di perpustakaan ini?</t>
+  </si>
+  <si>
+    <t>Apa saja layanan yang bisa digunakan di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu fasilitas umum perpustakaan.</t>
+  </si>
+  <si>
+    <t>Ada fasilitas pendukung di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Layanan umum apa saja yang ada di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Perpus ada wifi ga sih?</t>
+  </si>
+  <si>
+    <t>Mau tau dong fasilitas apa aja di perpus BIPA.</t>
+  </si>
+  <si>
+    <t>Cariin tempat nyaman buat ngerjain tugas di perpus.</t>
+  </si>
+  <si>
+    <t>Perpus BIPA ada tempat buat nongkrong sambil baca ga?</t>
+  </si>
+  <si>
+    <t>Bro, ada space buat diskusi kelompok di perpus?</t>
+  </si>
+  <si>
+    <t>Nyari quiet zone buat fokus belajar dimana ya?</t>
+  </si>
+  <si>
+    <t>Kasih tau gue fasilitas kece di perpus BIPA.</t>
+  </si>
+  <si>
+    <t>Pengen tau ruang baca dimana nih di perpus.</t>
+  </si>
+  <si>
+    <t>Bisa minjem komputer di perpus ga?</t>
+  </si>
+  <si>
+    <t>Tunjukin ruang multimedia di perpus BIPA.</t>
+  </si>
+  <si>
+    <t>Perpus punya printer ga sih?</t>
+  </si>
+  <si>
+    <t>Butuh tempat buat scan dokumen, perpus punya?</t>
+  </si>
+  <si>
+    <t>Ada gaak mesin fotokopi yang bisa dipake sendiri?</t>
+  </si>
+  <si>
+    <t>Di perpus BIPA boleh bawa minum ga?</t>
+  </si>
+  <si>
+    <t>Mau nitip tas dimana ya di perpus?</t>
+  </si>
+  <si>
+    <t>Caranya konek ke wifi perpus gimana nih?</t>
+  </si>
+  <si>
+    <t>Perpus ada colokan buat cas laptop ga?</t>
+  </si>
+  <si>
+    <t>Perpus BIPA nyediain headset buat pinjam ga?</t>
+  </si>
+  <si>
+    <t>Perpus BIPA punya e-book reader gak sih?</t>
+  </si>
+  <si>
+    <t>Buka dong info fasilitas perpus buat mahasiswa asing.</t>
+  </si>
+  <si>
+    <t>Ruang diskusi di perpus harus booking dulu ya?</t>
+  </si>
+  <si>
+    <t>Perpus ada pojok kopi gak? Pengen ngopi sambil baca nih.</t>
+  </si>
+  <si>
+    <t>Gw mau pake komputer perpus, caranya gimana?</t>
+  </si>
+  <si>
+    <t>Kasih tau jalan ke ruang audiovisual di perpus BIPA.</t>
+  </si>
+  <si>
+    <t>Ada sih locker di perpus buat nyimpen laptop?</t>
+  </si>
+  <si>
+    <t>Perpus BIPA ada ruang seminar ga ya?</t>
+  </si>
+  <si>
+    <t>Mesin fotokopi di perpus bisa dipake sendiri ga?</t>
+  </si>
+  <si>
+    <t>Nyalain AC dong di ruang baca, gerah nih.</t>
+  </si>
+  <si>
+    <t>Perpus BIPA ada layanan bimbingan penelusuran ga?</t>
+  </si>
+  <si>
+    <t>Gw butuh banget tempat sunyi, perpus ada ga?</t>
+  </si>
+  <si>
+    <t>Tunjukin dimana ruang referensi di perpus.</t>
+  </si>
+  <si>
+    <t>Ada bro, diskusi corner yang cozy di perpus?</t>
+  </si>
+  <si>
+    <t>Perpus ada toilet dimana sih?</t>
+  </si>
+  <si>
+    <t>Gak nemu nih tempat charging HP di perpus BIPA, bantuin dong.</t>
+  </si>
+  <si>
+    <t>Liat dong denah fasilitas perpus.</t>
+  </si>
+  <si>
+    <t>Perpus BIPA ada kursi yang empuk gak? Pegel duduk lama nih.</t>
+  </si>
+  <si>
+    <t>Cari ruang khusus buat video call di perpus.</t>
+  </si>
+  <si>
+    <t>Bro, perpus ada mini theater gak sih?</t>
+  </si>
+  <si>
+    <t>Perpus BIPA nyediain komputer buat riset ga?</t>
+  </si>
+  <si>
+    <t>Boleh makan snack di perpus gak ya?</t>
+  </si>
+  <si>
+    <t>Ada gak sih tempat diskusi yang kedap suara di perpus?</t>
+  </si>
+  <si>
+    <t>Perpus BIPA punya meja khusus buat gambar teknik?</t>
+  </si>
+  <si>
+    <t>Bantuin atur jadwal pake ruang multimedia di perpus.</t>
+  </si>
+  <si>
+    <t>Perpus ada standing desk gak? Capek duduk terus.</t>
+  </si>
+  <si>
+    <t>fasilitinya apa aja bang?</t>
+  </si>
+  <si>
+    <t>p ada wifi gx?</t>
+  </si>
+  <si>
+    <t>info baca dimana?</t>
+  </si>
+  <si>
+    <t>Gue butuh tempat diskusi bareng squad</t>
+  </si>
+  <si>
+    <t>info loker min</t>
+  </si>
+  <si>
+    <t>taruh jaket dmn?</t>
+  </si>
+  <si>
+    <t>boleh bawa tas?</t>
+  </si>
+  <si>
+    <t>Cari jurnal di sini bisa?</t>
+  </si>
+  <si>
+    <t>Butuh bantu cari skripsi.</t>
+  </si>
+  <si>
+    <t>Penelusuran literatur ada ya?</t>
+  </si>
+  <si>
+    <t>Skrpsi/jurnal tersedia?</t>
+  </si>
+  <si>
+    <t>Mau fotokopi koleksi.</t>
+  </si>
+  <si>
+    <t>Cari ruang baca.</t>
+  </si>
+  <si>
+    <t>Ruang baca free kah?</t>
+  </si>
+  <si>
+    <t>Ada ruangan buat baca?</t>
+  </si>
+  <si>
+    <t>Locker tas tersedia?</t>
+  </si>
+  <si>
+    <t>Titip tas di mana?</t>
+  </si>
+  <si>
+    <t>Ada locker buat jaket?</t>
+  </si>
+  <si>
+    <t>Internet gratis kan?</t>
+  </si>
+  <si>
+    <t>Pakai WiFi gimana?</t>
+  </si>
+  <si>
+    <t>Minta akses WiFi.</t>
+  </si>
+  <si>
+    <t>Fasilitas lengkap apa aja?</t>
+  </si>
+  <si>
+    <t>sebutkan semua fasilitas disini</t>
+  </si>
+  <si>
+    <t>di Perpus ada alat bantu baca gak buat yang low vision?</t>
+  </si>
+  <si>
+    <t>perpustakaan stmik bina patria fiturnya apa aja min?</t>
+  </si>
+  <si>
+    <t>info kelengkapan perpus</t>
+  </si>
+  <si>
+    <t>berikan saya daftar fasility</t>
+  </si>
+  <si>
+    <t>dapatkan semua fasilitas disini</t>
+  </si>
+  <si>
+    <t>woy kasih tau gw semua benda di perpus</t>
   </si>
 </sst>
 </file>
@@ -3497,16 +3845,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C876"/>
+  <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A848" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A1001" sqref="A1001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="93.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -10524,9 +10872,1009 @@
         <v>755</v>
       </c>
     </row>
+    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>949</v>
+      </c>
+      <c r="B877" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>897</v>
+      </c>
+      <c r="B878" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>910</v>
+      </c>
+      <c r="B879" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>916</v>
+      </c>
+      <c r="B880" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>893</v>
+      </c>
+      <c r="B881" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>875</v>
+      </c>
+      <c r="B882" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>875</v>
+      </c>
+      <c r="B883" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>930</v>
+      </c>
+      <c r="B884" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>958</v>
+      </c>
+      <c r="B885" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>979</v>
+      </c>
+      <c r="B886" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>906</v>
+      </c>
+      <c r="B887" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>901</v>
+      </c>
+      <c r="B888" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>886</v>
+      </c>
+      <c r="B889" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>882</v>
+      </c>
+      <c r="B890" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>882</v>
+      </c>
+      <c r="B891" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>976</v>
+      </c>
+      <c r="B892" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>942</v>
+      </c>
+      <c r="B893" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>887</v>
+      </c>
+      <c r="B894" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>914</v>
+      </c>
+      <c r="B895" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>908</v>
+      </c>
+      <c r="B896" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>894</v>
+      </c>
+      <c r="B897" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>903</v>
+      </c>
+      <c r="B898" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>898</v>
+      </c>
+      <c r="B899" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
+        <v>878</v>
+      </c>
+      <c r="B900" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
+        <v>878</v>
+      </c>
+      <c r="B901" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
+        <v>891</v>
+      </c>
+      <c r="B902" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>880</v>
+      </c>
+      <c r="B903" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>880</v>
+      </c>
+      <c r="B904" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>911</v>
+      </c>
+      <c r="B905" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>960</v>
+      </c>
+      <c r="B906" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>884</v>
+      </c>
+      <c r="B907" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>884</v>
+      </c>
+      <c r="B908" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>909</v>
+      </c>
+      <c r="B909" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>905</v>
+      </c>
+      <c r="B910" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>926</v>
+      </c>
+      <c r="B911" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>968</v>
+      </c>
+      <c r="B912" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
+        <v>957</v>
+      </c>
+      <c r="B913" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>902</v>
+      </c>
+      <c r="B914" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A915" t="s">
+        <v>922</v>
+      </c>
+      <c r="B915" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A916" t="s">
+        <v>955</v>
+      </c>
+      <c r="B916" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
+        <v>937</v>
+      </c>
+      <c r="B917" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
+        <v>970</v>
+      </c>
+      <c r="B918" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A919" t="s">
+        <v>929</v>
+      </c>
+      <c r="B919" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A920" t="s">
+        <v>933</v>
+      </c>
+      <c r="B920" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A921" t="s">
+        <v>969</v>
+      </c>
+      <c r="B921" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A922" t="s">
+        <v>974</v>
+      </c>
+      <c r="B922" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A923" t="s">
+        <v>954</v>
+      </c>
+      <c r="B923" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A924" t="s">
+        <v>920</v>
+      </c>
+      <c r="B924" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
+        <v>904</v>
+      </c>
+      <c r="B925" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
+        <v>931</v>
+      </c>
+      <c r="B926" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
+        <v>892</v>
+      </c>
+      <c r="B927" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
+        <v>900</v>
+      </c>
+      <c r="B928" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>896</v>
+      </c>
+      <c r="B929" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>913</v>
+      </c>
+      <c r="B930" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A931" t="s">
+        <v>876</v>
+      </c>
+      <c r="B931" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A932" t="s">
+        <v>876</v>
+      </c>
+      <c r="B932" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>983</v>
+      </c>
+      <c r="B933" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A934" t="s">
+        <v>885</v>
+      </c>
+      <c r="B934" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A935" t="s">
+        <v>962</v>
+      </c>
+      <c r="B935" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A936" t="s">
+        <v>951</v>
+      </c>
+      <c r="B936" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>965</v>
+      </c>
+      <c r="B937" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>947</v>
+      </c>
+      <c r="B938" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>940</v>
+      </c>
+      <c r="B939" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>964</v>
+      </c>
+      <c r="B940" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>966</v>
+      </c>
+      <c r="B941" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>980</v>
+      </c>
+      <c r="B942" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>912</v>
+      </c>
+      <c r="B943" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A944" t="s">
+        <v>888</v>
+      </c>
+      <c r="B944" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A945" t="s">
+        <v>924</v>
+      </c>
+      <c r="B945" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A946" t="s">
+        <v>941</v>
+      </c>
+      <c r="B946" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A947" t="s">
+        <v>917</v>
+      </c>
+      <c r="B947" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A948" t="s">
+        <v>952</v>
+      </c>
+      <c r="B948" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A949" t="s">
+        <v>907</v>
+      </c>
+      <c r="B949" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A950" t="s">
+        <v>977</v>
+      </c>
+      <c r="B950" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A951" t="s">
+        <v>973</v>
+      </c>
+      <c r="B951" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A952" t="s">
+        <v>932</v>
+      </c>
+      <c r="B952" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>919</v>
+      </c>
+      <c r="B953" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A954" t="s">
+        <v>944</v>
+      </c>
+      <c r="B954" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A955" t="s">
+        <v>982</v>
+      </c>
+      <c r="B955" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A956" t="s">
+        <v>945</v>
+      </c>
+      <c r="B956" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A957" t="s">
+        <v>923</v>
+      </c>
+      <c r="B957" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A958" t="s">
+        <v>963</v>
+      </c>
+      <c r="B958" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A959" t="s">
+        <v>981</v>
+      </c>
+      <c r="B959" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A960" t="s">
+        <v>971</v>
+      </c>
+      <c r="B960" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A961" t="s">
+        <v>925</v>
+      </c>
+      <c r="B961" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A962" t="s">
+        <v>934</v>
+      </c>
+      <c r="B962" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A963" t="s">
+        <v>939</v>
+      </c>
+      <c r="B963" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A964" t="s">
+        <v>961</v>
+      </c>
+      <c r="B964" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A965" t="s">
+        <v>950</v>
+      </c>
+      <c r="B965" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A966" t="s">
+        <v>918</v>
+      </c>
+      <c r="B966" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A967" t="s">
+        <v>985</v>
+      </c>
+      <c r="B967" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A968" t="s">
+        <v>953</v>
+      </c>
+      <c r="B968" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A969" t="s">
+        <v>946</v>
+      </c>
+      <c r="B969" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A970" t="s">
+        <v>943</v>
+      </c>
+      <c r="B970" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A971" t="s">
+        <v>921</v>
+      </c>
+      <c r="B971" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A972" t="s">
+        <v>935</v>
+      </c>
+      <c r="B972" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A973" t="s">
+        <v>956</v>
+      </c>
+      <c r="B973" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A974" t="s">
+        <v>936</v>
+      </c>
+      <c r="B974" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A975" t="s">
+        <v>959</v>
+      </c>
+      <c r="B975" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A976" t="s">
+        <v>928</v>
+      </c>
+      <c r="B976" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A977" t="s">
+        <v>883</v>
+      </c>
+      <c r="B977" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="978" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A978" t="s">
+        <v>883</v>
+      </c>
+      <c r="B978" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="979" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>895</v>
+      </c>
+      <c r="B979" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>879</v>
+      </c>
+      <c r="B980" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="981" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>879</v>
+      </c>
+      <c r="B981" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>975</v>
+      </c>
+      <c r="B982" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>938</v>
+      </c>
+      <c r="B983" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="984" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>889</v>
+      </c>
+      <c r="B984" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>881</v>
+      </c>
+      <c r="B985" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="986" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>881</v>
+      </c>
+      <c r="B986" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="987" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>915</v>
+      </c>
+      <c r="B987" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="988" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>899</v>
+      </c>
+      <c r="B988" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="989" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>877</v>
+      </c>
+      <c r="B989" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>877</v>
+      </c>
+      <c r="B990" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="991" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>984</v>
+      </c>
+      <c r="B991" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="992" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
+        <v>972</v>
+      </c>
+      <c r="B992" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="993" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A993" t="s">
+        <v>967</v>
+      </c>
+      <c r="B993" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="994" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A994" t="s">
+        <v>978</v>
+      </c>
+      <c r="B994" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="995" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A995" t="s">
+        <v>948</v>
+      </c>
+      <c r="B995" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="996" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A996" t="s">
+        <v>927</v>
+      </c>
+      <c r="B996" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="997" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>986</v>
+      </c>
+      <c r="B997" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="998" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
+        <v>987</v>
+      </c>
+      <c r="B998" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="999" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A999" t="s">
+        <v>988</v>
+      </c>
+      <c r="B999" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1000" t="s">
+        <v>989</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1001" t="s">
+        <v>990</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>890</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:B876">
-    <sortCondition ref="B1:B876"/>
+  <sortState ref="A877:B1002">
+    <sortCondition ref="A877:A1002"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add new intent, pinjam_buku
</commit_message>
<xml_diff>
--- a/train.xlsx
+++ b/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChatbotPerpusBipa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782469EE-3D7E-40D7-A95D-E17674A2A7AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4167B4A-4D90-42D4-B3F9-EA3A2EC8C949}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Book1!$A$2:$B$1002</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Book1!$A$1002:$A$1012</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="1002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="1127">
   <si>
     <t>text</t>
   </si>
@@ -3036,13 +3036,388 @@
   </si>
   <si>
     <t>permisi selamat siang, saya baru, tolong jelaskan semua sarana di perpustakaan ini, terima kasih</t>
+  </si>
+  <si>
+    <t>Bagaimanakah prosedur peminjaman buku di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Mohon informasinya terkait tata cara meminjam buku.</t>
+  </si>
+  <si>
+    <t>Saya ingin mengetahui cara peminjaman buku yang benar.</t>
+  </si>
+  <si>
+    <t>Apa saja syarat dan ketentuan untuk meminjam buku?</t>
+  </si>
+  <si>
+    <t>Dapatkah Anda menjelaskan langkah-langkah meminjam buku?</t>
+  </si>
+  <si>
+    <t>Tolong beritahu prosedur resmi peminjaman buku di sini.</t>
+  </si>
+  <si>
+    <t>cara_pinjam</t>
+  </si>
+  <si>
+    <t>Gue mau minjem buku, tapi belum tau caranya.</t>
+  </si>
+  <si>
+    <t>Minjem buku di sini kayak gimana ya?</t>
+  </si>
+  <si>
+    <t>Jadi kalau mau pinjem buku harus ngapain dulu?</t>
+  </si>
+  <si>
+    <t>Gimana sih cara minjem buku di perpus?</t>
+  </si>
+  <si>
+    <t>Kalau mau pinjam buku tuh ngapain aja?</t>
+  </si>
+  <si>
+    <t>Bisa pinjem buku nggak? Caranya gimana?</t>
+  </si>
+  <si>
+    <t>Gimana prosedur pinjam-pinjam buku di sini?</t>
+  </si>
+  <si>
+    <t>Apa langkah pertama buat pinjam buku?</t>
+  </si>
+  <si>
+    <t>Jelaskan proses peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Bisa nggak dijelasin cara pinjam buku?</t>
+  </si>
+  <si>
+    <t>Tolong kasih tahu step by step peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Apa yang harus saya lakukan untuk bisa meminjam buku?</t>
+  </si>
+  <si>
+    <t>Saya belum pernah pinjam buku, jadi masih bingung caranya.</t>
+  </si>
+  <si>
+    <t>Kalau belum pernah pinjam buku, harus mulai dari mana?</t>
+  </si>
+  <si>
+    <t>Katanya bisa pinjam buku di sini, gimana ya?</t>
+  </si>
+  <si>
+    <t>Ada aturan khusus nggak buat pinjam buku?</t>
+  </si>
+  <si>
+    <t>Mau tanya soal cara pinjam buku dong.</t>
+  </si>
+  <si>
+    <t>Minjem buku tuh rules-nya gimana ya?</t>
+  </si>
+  <si>
+    <t>Auto pinjem buku tuh bisa dari HP nggak sih?</t>
+  </si>
+  <si>
+    <t>Ada tutorial pinjem buku gitu nggak?</t>
+  </si>
+  <si>
+    <t>Mau pinjem buku nih, kasih tau triknya dong.</t>
+  </si>
+  <si>
+    <t>Newbie nih, cara pinjem buku di perpus kampus gimana?</t>
+  </si>
+  <si>
+    <t>Saya boleh pinjam buku? Tapi belum tahu caranya.</t>
+  </si>
+  <si>
+    <t>Pinjam buku bisa, kan? Tapi harus daftar dulu ya?</t>
+  </si>
+  <si>
+    <t>Saya baru pertama kali, boleh minta panduannya?</t>
+  </si>
+  <si>
+    <t>Caranya ribet nggak buat pinjam buku?</t>
+  </si>
+  <si>
+    <t>Harus jadi anggota dulu kah kalau mau pinjam?</t>
+  </si>
+  <si>
+    <t>Bagaimana proses pengambilan buku di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Kalau ingin meminjam koleksi buku, syaratnya apa?</t>
+  </si>
+  <si>
+    <t>Apa mekanisme peminjaman buku di sini?</t>
+  </si>
+  <si>
+    <t>Untuk meminjam bahan bacaan, prosedurnya apa saja?</t>
+  </si>
+  <si>
+    <t>Gimana alur pinjam buku di sistem ini?</t>
+  </si>
+  <si>
+    <t>Saya pengen pinjam buku, tapi belum tahu caranya. Bisa bantu?</t>
+  </si>
+  <si>
+    <t>Kalau saya mau pinjam buku, harus ngapain dulu ya?</t>
+  </si>
+  <si>
+    <t>Cara pinjam buku?</t>
+  </si>
+  <si>
+    <t>Mau pinjam buku.</t>
+  </si>
+  <si>
+    <t>Gimana pinjamnya?</t>
+  </si>
+  <si>
+    <t>Prosedur pinjam buku?</t>
+  </si>
+  <si>
+    <t>Langkah pinjam buku?</t>
+  </si>
+  <si>
+    <t>Syarat pinjam buku?</t>
+  </si>
+  <si>
+    <t>Boleh pinjam buku?</t>
+  </si>
+  <si>
+    <t>Pinjam buku gimana?</t>
+  </si>
+  <si>
+    <t>Pinjam buku dong.</t>
+  </si>
+  <si>
+    <t>Buku bisa dipinjam?</t>
+  </si>
+  <si>
+    <t>Jelaskan prosedur meminjam buku.</t>
+  </si>
+  <si>
+    <t>Tunjukkan cara pinjam buku.</t>
+  </si>
+  <si>
+    <t>Pandu saya untuk pinjam buku.</t>
+  </si>
+  <si>
+    <t>Tolong informasikan cara peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Tulis langkah-langkah peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Kasih tahu saya cara meminjam buku.</t>
+  </si>
+  <si>
+    <t>Tolong sampaikan prosedurnya.</t>
+  </si>
+  <si>
+    <t>Beritahu saya proses pinjam buku.</t>
+  </si>
+  <si>
+    <t>Jelaskan dari awal sampai akhir.</t>
+  </si>
+  <si>
+    <t>Buat saya ngerti cara pinjam buku.</t>
+  </si>
+  <si>
+    <t>Saya belum tahu cara pinjam buku.</t>
+  </si>
+  <si>
+    <t>Saya bingung gimana pinjam buku.</t>
+  </si>
+  <si>
+    <t>Saya butuh informasi soal peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Belum ngerti prosedur pinjam buku.</t>
+  </si>
+  <si>
+    <t>Belum pernah pinjam buku, jadi butuh panduan.</t>
+  </si>
+  <si>
+    <t>Mau pinjam buku tapi nggak tahu caranya.</t>
+  </si>
+  <si>
+    <t>Pertama kali mau pinjam buku.</t>
+  </si>
+  <si>
+    <t>Niatnya sih pinjam buku, tapi belum paham langkah-langkahnya.</t>
+  </si>
+  <si>
+    <t>Sepertinya ada prosedur buat pinjam buku.</t>
+  </si>
+  <si>
+    <t>Bingung cara pinjam buku di sini.</t>
+  </si>
+  <si>
+    <t>Eh, kalau mau pinjam buku ngapain aja sih?</t>
+  </si>
+  <si>
+    <t>Jadi prosedurnya gimana nih?</t>
+  </si>
+  <si>
+    <t>Gue ke sini buat pinjam buku, tapi bingung.</t>
+  </si>
+  <si>
+    <t>Minjem buku bisa langsung atau harus daftar dulu?</t>
+  </si>
+  <si>
+    <t>Yang bener tuh pinjamnya lewat mana?</t>
+  </si>
+  <si>
+    <t>Jadi, ke petugas langsung aja gitu?</t>
+  </si>
+  <si>
+    <t>Harus login dulu kalau mau pinjam ya?</t>
+  </si>
+  <si>
+    <t>Ada batas maksimal pinjam buku nggak sih?</t>
+  </si>
+  <si>
+    <t>Boleh bantuin jelasin pinjam buku?</t>
+  </si>
+  <si>
+    <t>Gak ngerti sistem peminjaman di sini.</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu prosedur peminjaman.</t>
+  </si>
+  <si>
+    <t>Tolong berikan informasi peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Saya perlu bantuan soal peminjaman buku.</t>
+  </si>
+  <si>
+    <t>Boleh dijelaskan langkah pinjam buku?</t>
+  </si>
+  <si>
+    <t>Saya sedang mencari tahu cara pinjam buku.</t>
+  </si>
+  <si>
+    <t>selamat oagi bang!,  kalo mau pinjam buku caranya gmn</t>
+  </si>
+  <si>
+    <t>cara pinjam, terima kasih!</t>
+  </si>
+  <si>
+    <t>saya pengen minjem, apakah ada aturan tertentu?</t>
+  </si>
+  <si>
+    <t>minjem buku kapan kembalinya?</t>
+  </si>
+  <si>
+    <t>maksimal boleh pinjem berapa</t>
+  </si>
+  <si>
+    <t>Kapan batas maksimal pengembalian buku?</t>
+  </si>
+  <si>
+    <t>Berapa lama buku boleh dipinjam?</t>
+  </si>
+  <si>
+    <t>Berapa jumlah buku yang bisa saya pinjam sekaligus?</t>
+  </si>
+  <si>
+    <t>Ada denda nggak kalau telat balikin buku?</t>
+  </si>
+  <si>
+    <t>Pinjam buku maksimal berapa hari?</t>
+  </si>
+  <si>
+    <t>Satu orang boleh pinjam berapa buku?</t>
+  </si>
+  <si>
+    <t>Apakah harus jadi anggota dulu untuk bisa meminjam?</t>
+  </si>
+  <si>
+    <t>Bisa pinjam buku tanpa kartu anggota nggak?</t>
+  </si>
+  <si>
+    <t>Buku referensi bisa dipinjam juga?</t>
+  </si>
+  <si>
+    <t>Pengembalian bukunya ke mana ya?</t>
+  </si>
+  <si>
+    <t>Ada batasan jenis buku yang bisa dipinjam?</t>
+  </si>
+  <si>
+    <t>Peminjaman bisa dilakukan secara online?</t>
+  </si>
+  <si>
+    <t>Kalau bukunya hilang, gimana prosesnya?</t>
+  </si>
+  <si>
+    <t>Perlu konfirmasi dulu sebelum pinjam?</t>
+  </si>
+  <si>
+    <t>Kalau buku sedang dipinjam orang lain, bisa antri?</t>
+  </si>
+  <si>
+    <t>batas peminjaman</t>
+  </si>
+  <si>
+    <t>maksimum pinjam</t>
+  </si>
+  <si>
+    <t>boleh ga pinjem 4 buku?</t>
+  </si>
+  <si>
+    <t>selamat sore, apakah boleh meminjam banyak buku sekaligus?</t>
+  </si>
+  <si>
+    <t>halo, selamat malam, jelaskan cara meminjam buku diperpus</t>
+  </si>
+  <si>
+    <t>buku appa aja yang boleh dipinjem?</t>
+  </si>
+  <si>
+    <t>apakah buku harus dikembalikan tepat waktu?</t>
+  </si>
+  <si>
+    <t>selamat siang, ada prosedur peminjaman dan pengembalian buku?</t>
+  </si>
+  <si>
+    <t>p, cara minjem buku</t>
+  </si>
+  <si>
+    <t>woigh cara pinjeman buku</t>
+  </si>
+  <si>
+    <t>how to borrow a book</t>
+  </si>
+  <si>
+    <t>saya ingin borrow buuku</t>
+  </si>
+  <si>
+    <t>apakah boleh telat beberapa hari?</t>
+  </si>
+  <si>
+    <t>permisi, adakah daftar aturan pinjam buku</t>
+  </si>
+  <si>
+    <t>show me, tata cara peminjaman di perpustakaan stmik bina patria</t>
+  </si>
+  <si>
+    <t>apa aja hal hal yang harus saya ketahui saat meminjam</t>
+  </si>
+  <si>
+    <t>kalo telat sehari boleh ga?</t>
+  </si>
+  <si>
+    <t>bukunya boleh dibaca diluar?</t>
+  </si>
+  <si>
+    <t>bukunya boleh dibawa pulang gx?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3173,14 +3548,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3532,7 +3899,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3888,10 +4257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1001"/>
+  <dimension ref="A1:C1126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C499" sqref="C499"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3899,10 +4268,10 @@
     <col min="1" max="1" width="100.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3910,43 +4279,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>607</v>
       </c>
       <c r="B2" t="s">
         <v>516</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>612</v>
       </c>
       <c r="B3" t="s">
         <v>516</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>621</v>
       </c>
       <c r="B4" t="s">
         <v>516</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>590</v>
       </c>
       <c r="B5" t="s">
         <v>516</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>523</v>
       </c>
@@ -3954,7 +4319,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>550</v>
       </c>
@@ -3962,7 +4327,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>627</v>
       </c>
@@ -3970,7 +4335,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>541</v>
       </c>
@@ -3978,7 +4343,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>556</v>
       </c>
@@ -3986,7 +4351,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>566</v>
       </c>
@@ -3994,7 +4359,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>617</v>
       </c>
@@ -4002,7 +4367,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>568</v>
       </c>
@@ -4010,7 +4375,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>530</v>
       </c>
@@ -4018,7 +4383,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>593</v>
       </c>
@@ -4026,7 +4391,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>570</v>
       </c>
@@ -11920,9 +12285,1009 @@
         <v>739</v>
       </c>
     </row>
+    <row r="1002" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1002" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1003" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1004" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1005" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1006" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1007" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1008" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1009" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1010" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1011" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1012" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1013" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1014" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1015" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1016" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1017" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1018" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1019" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1020" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1021" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1022" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1023" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1024" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1025" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1026" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1027" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1028" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1029" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1030" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1031" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1032" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1033" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1034" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1035" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1036" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1037" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1038" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1039" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1040" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1041" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1042" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1043" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1044" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1045" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1046" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1047" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1048" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1049" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1050" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1051" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1052" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1053" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1054" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1055" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1056" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1059" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1060" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1061" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1062" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1063" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1064" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1065" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1066" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1067" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1068" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1069" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1070" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1071" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1072" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1073" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1074" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1075" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1076" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1077" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1078" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1079" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1080" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1081" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1082" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1083" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1084" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1085" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1086" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1087" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1088" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1089" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1090" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1091" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1092" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1093" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1094" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1095" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1096" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1097" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1098" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1099" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1100" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1101" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1102" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1104" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1105" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1106" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1107" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1108" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1109" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1111" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1112" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1113" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1114" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1115" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1116" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1117" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1118" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1119" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1120" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1121" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1122" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1123" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1124" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1125" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1126" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>1008</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A377:B501">
-    <sortCondition ref="A377:A501"/>
+  <sortState ref="A1092:A1120">
+    <sortCondition ref="A1092"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add new intent datasets
</commit_message>
<xml_diff>
--- a/train.xlsx
+++ b/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChatbotPerpusBipa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4167B4A-4D90-42D4-B3F9-EA3A2EC8C949}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472078DD-CF7D-4207-A906-62E7980487DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="1253">
   <si>
     <t>text</t>
   </si>
@@ -3411,6 +3411,384 @@
   </si>
   <si>
     <t>bukunya boleh dibawa pulang gx?</t>
+  </si>
+  <si>
+    <t>peraturan</t>
+  </si>
+  <si>
+    <t>apa saja aturanya in</t>
+  </si>
+  <si>
+    <t>halo , saya baru disini, apa saja aturan di perpus bipa?</t>
+  </si>
+  <si>
+    <t>info peraturan</t>
+  </si>
+  <si>
+    <t>infokan tata tertib</t>
+  </si>
+  <si>
+    <t>apa saja rules yang berlaku disini?</t>
+  </si>
+  <si>
+    <t>ketentuan tata tertib</t>
+  </si>
+  <si>
+    <t>rulesnya apa aja coy</t>
+  </si>
+  <si>
+    <t>spill list peraturan</t>
+  </si>
+  <si>
+    <t>apa saja kebijakan disini?</t>
+  </si>
+  <si>
+    <t>Apa aja sih aturan di perpustakaan ini?</t>
+  </si>
+  <si>
+    <t>Bisa kasih tahu peraturan yang berlaku?</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu tata tertib di sini</t>
+  </si>
+  <si>
+    <t>Ada daftar peraturan yang bisa saya lihat?</t>
+  </si>
+  <si>
+    <t>Mohon info tentang kebijakan perpustakaan</t>
+  </si>
+  <si>
+    <t>Aturan main di perpustakaan gimana ya?</t>
+  </si>
+  <si>
+    <t>Boleh minta list tata tertibnya?</t>
+  </si>
+  <si>
+    <t>Perpustakaan ini ada peraturannya nggak?</t>
+  </si>
+  <si>
+    <t>Ketentuan yang harus dipatuhi apa aja?</t>
+  </si>
+  <si>
+    <t>Peraturan pengunjung apa aja?</t>
+  </si>
+  <si>
+    <t>Info tata tertib dong</t>
+  </si>
+  <si>
+    <t>Pengen tahu aturan kalau mau pakai layanan di sini</t>
+  </si>
+  <si>
+    <t>Ada SOP atau peraturan resmi kah?</t>
+  </si>
+  <si>
+    <t>Rulesnya apa aja bro?</t>
+  </si>
+  <si>
+    <t>Peraturan di BIPA gimana?</t>
+  </si>
+  <si>
+    <t>Gue harus tahu dulu aturannya nih</t>
+  </si>
+  <si>
+    <t>Ada larangan khusus gak di perpus ini?</t>
+  </si>
+  <si>
+    <t>Kasih tahu dong kebijakan yang berlaku</t>
+  </si>
+  <si>
+    <t>Perlu taat sama aturan apa aja di sini?</t>
+  </si>
+  <si>
+    <t>Aturan peminjaman dan penggunaan tempatnya gimana?</t>
+  </si>
+  <si>
+    <t>Syarat dan ketentuan di sini apa?</t>
+  </si>
+  <si>
+    <t>Gimana prosedur dan aturannya?</t>
+  </si>
+  <si>
+    <t>Hal-hal yang gak boleh dilakukan apa aja?</t>
+  </si>
+  <si>
+    <t>Apa ada panduan buat pengunjung baru?</t>
+  </si>
+  <si>
+    <t>Saya harus tahu dulu peraturannya sebelum mulai pakai</t>
+  </si>
+  <si>
+    <t>Mohon informasikan tata tertib di BIPA</t>
+  </si>
+  <si>
+    <t>Bisa dijelaskan peraturan-peraturan yang berlaku?</t>
+  </si>
+  <si>
+    <t>Aturan untuk pengunjung baru seperti saya apa aja?</t>
+  </si>
+  <si>
+    <t>Boleh minta info tentang regulasi perpus ini?</t>
+  </si>
+  <si>
+    <t>Share dong peraturan dasar di sini</t>
+  </si>
+  <si>
+    <t>Hal-hal yang harus dipatuhi apa saja?</t>
+  </si>
+  <si>
+    <t>Dilarang ngapain aja di perpus?</t>
+  </si>
+  <si>
+    <t>Spill dong semua peraturannya</t>
+  </si>
+  <si>
+    <t>Ada poster atau dokumen yang berisi peraturan?</t>
+  </si>
+  <si>
+    <t>Aturan berpakaian dan bersikap gimana?</t>
+  </si>
+  <si>
+    <t>Ada jam-jam tertentu yang diatur?</t>
+  </si>
+  <si>
+    <t>Boleh bawa makanan? Atau ada aturannya?</t>
+  </si>
+  <si>
+    <t>Bisa bantu jelaskan ketentuan umum di sini?</t>
+  </si>
+  <si>
+    <t>Saya pengunjung baru, boleh tahu rules-nya?</t>
+  </si>
+  <si>
+    <t>Aturan penggunaan komputer dan fasilitas lainnya gimana?</t>
+  </si>
+  <si>
+    <t>Saya butuh tahu peraturan dulu sebelum gabung</t>
+  </si>
+  <si>
+    <t>Tata tertib buat anggota dan non-anggota sama gak?</t>
+  </si>
+  <si>
+    <t>Wajib patuh sama aturan tertentu kah?</t>
+  </si>
+  <si>
+    <t>Peraturan penting yang harus diketahui apa?</t>
+  </si>
+  <si>
+    <t>List larangan dan keharusan di sini dong</t>
+  </si>
+  <si>
+    <t>Boleh dijelasin panduan umumnya?</t>
+  </si>
+  <si>
+    <t>Hal-hal yang dianggap melanggar apa aja?</t>
+  </si>
+  <si>
+    <t>Gimana prosedur kalau melanggar peraturan?</t>
+  </si>
+  <si>
+    <t>Sanksinya apa kalau melanggar aturan?</t>
+  </si>
+  <si>
+    <t>Ada kebijakan khusus yang harus saya tahu?</t>
+  </si>
+  <si>
+    <t>sebutkan kebijakan kebijakan disini</t>
+  </si>
+  <si>
+    <t>Tolong jelaskan aturan perpustakaan</t>
+  </si>
+  <si>
+    <t>Apa peraturan di perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Ketentuan perpustakaan apa saja?</t>
+  </si>
+  <si>
+    <t>Boleh minta informasi tata tertib perpustakaan?</t>
+  </si>
+  <si>
+    <t>Rules perpustakaan BIPA dong</t>
+  </si>
+  <si>
+    <t>Ada peraturan khusus di perpus ini?</t>
+  </si>
+  <si>
+    <t>Perpustakaan ini punya aturan apa saja ya?</t>
+  </si>
+  <si>
+    <t>Kebijakan perpustakaan seperti apa?</t>
+  </si>
+  <si>
+    <t>Saya mau tahu aturan perpustakaan</t>
+  </si>
+  <si>
+    <t>Standar operasional perpustakaan apa saja?</t>
+  </si>
+  <si>
+    <t>Panduan penggunaan perpustakaan untuk pemula</t>
+  </si>
+  <si>
+    <t>Aturan yang harus dipatuhi di perpus apa aja?</t>
+  </si>
+  <si>
+    <t>Apa tata tertib di perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Butuh info tentang aturan perpustakaan</t>
+  </si>
+  <si>
+    <t>Berikan penjelasan tentang kebijakan perpustakaan</t>
+  </si>
+  <si>
+    <t>Mau tanya soal peraturan perpusnya</t>
+  </si>
+  <si>
+    <t>Aturan peminjaman buku gimana ya?</t>
+  </si>
+  <si>
+    <t>Kewajiban pengunjung perpustakaan apa saja?</t>
+  </si>
+  <si>
+    <t>Aturan main di perpus BIPA dong</t>
+  </si>
+  <si>
+    <t>Apa saja yang dilarang di perpustakaan ini?</t>
+  </si>
+  <si>
+    <t>Tata tertib penggunaan perpustakaan</t>
+  </si>
+  <si>
+    <t>Boleh tahu aturan perpustakaan untuk pengunjung?</t>
+  </si>
+  <si>
+    <t>Jelaskan tata tertib perpustakaan dong</t>
+  </si>
+  <si>
+    <t>Peraturan yang berlaku di perpus ini apa saja?</t>
+  </si>
+  <si>
+    <t>Sistem aturan perpustakaan seperti apa?</t>
+  </si>
+  <si>
+    <t>Mau tahu tentang peraturan di perpus BIPA</t>
+  </si>
+  <si>
+    <t>Aturan dan tata cara di perpustakaan</t>
+  </si>
+  <si>
+    <t>Apa regulasi yang berlaku di perpus ini?</t>
+  </si>
+  <si>
+    <t>Ketentuannya apa aja di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Aturan perpus yang perlu ditaati</t>
+  </si>
+  <si>
+    <t>Apa ada peraturan khusus di perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Tolong kasih info tentang tata tertib perpus</t>
+  </si>
+  <si>
+    <t>Bisakah dijelaskan peraturan perpustakaannya?</t>
+  </si>
+  <si>
+    <t>Ketentuan yang ada di perpustakaan ini</t>
+  </si>
+  <si>
+    <t>Perpustakaan BIPA punya aturan apa?</t>
+  </si>
+  <si>
+    <t>Regulasi perpustakaan gimana ya?</t>
+  </si>
+  <si>
+    <t>Pedoman di perpustakaan apa saja?</t>
+  </si>
+  <si>
+    <t>Aturan standar perpustakaan gimana?</t>
+  </si>
+  <si>
+    <t>Apa ada kebijakan spesifik di perpustakaan?</t>
+  </si>
+  <si>
+    <t>Kasih tau dong aturan perpusnya</t>
+  </si>
+  <si>
+    <t>Peraturannya gimana di perpus BIPA?</t>
+  </si>
+  <si>
+    <t>Mau tahu prosedur dan ketentuan perpustakaan</t>
+  </si>
+  <si>
+    <t>Tata tertib yang berlaku di perpustakaan</t>
+  </si>
+  <si>
+    <t>Apa yang tidak boleh dilakukan di perpus?</t>
+  </si>
+  <si>
+    <t>Aturan buat pengunjung perpustakaan baru</t>
+  </si>
+  <si>
+    <t>Peraturan kerja di perpustakaan</t>
+  </si>
+  <si>
+    <t>Aturan penggunaan fasilitas perpustakaan</t>
+  </si>
+  <si>
+    <t>Apa kebijakan perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Aturan perpus yang wajib ditaati</t>
+  </si>
+  <si>
+    <t>Kebijakan operasional perpustakaan</t>
+  </si>
+  <si>
+    <t>Jelaskan aturan dasar perpustakaan dong</t>
+  </si>
+  <si>
+    <t>Aturan perpustakaan untuk pemula</t>
+  </si>
+  <si>
+    <t>Apa saja larangan di perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Peraturan teknis perpustakaan seperti apa?</t>
+  </si>
+  <si>
+    <t>Ketentuan penggunaan perpustakaan</t>
+  </si>
+  <si>
+    <t>Panduan peraturan perpus buat pengunjung</t>
+  </si>
+  <si>
+    <t>Aturan peminjaman di perpustakaan BIPA?</t>
+  </si>
+  <si>
+    <t>Rules yang berlaku di perpus ini apa?</t>
+  </si>
+  <si>
+    <t>Butuh informasi tentang kebijakan perpustakaan</t>
+  </si>
+  <si>
+    <t>Ada dokumen peraturan perpustakaan?</t>
+  </si>
+  <si>
+    <t>Kebijakan untuk pengunjung perpustakaan</t>
+  </si>
+  <si>
+    <t>Tata tertib perpustakaan BIPA apa saja?</t>
+  </si>
+  <si>
+    <t>Aturan yang wajib diikuti di perpustakaan</t>
+  </si>
+  <si>
+    <t>Apa peraturan resmi perpustakaan?</t>
+  </si>
+  <si>
+    <t>Selamat sore, daftar peraturan yang tidak boleh dilanggar apa saja? Makasih</t>
   </si>
 </sst>
 </file>
@@ -4257,10 +4635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1126"/>
+  <dimension ref="A1:C1251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A1238" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A1261" sqref="A1261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13285,9 +13663,1009 @@
         <v>1008</v>
       </c>
     </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1127" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1128" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1129" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1130" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1131" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1132" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1133" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1134" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1135" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1136" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1137" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1138" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1139" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1140" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1141" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1142" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1143" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1144" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1145" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1146" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1147" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1148" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1149" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1150" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1151" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1152" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1153" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1154" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1155" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1156" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1157" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1158" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1159" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1160" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1161" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1162" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1163" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1164" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1165" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1166" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1167" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1168" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1169" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1170" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1171" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1172" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1173" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1174" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1175" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1176" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1177" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1178" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1179" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1180" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1181" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1182" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1183" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1184" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1185" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1186" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1187" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1188" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1189" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1190" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1191" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1192" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1193" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1194" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1195" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1196" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1197" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1198" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1199" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1200" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1201" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1202" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1203" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1204" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1205" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1206" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1207" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1208" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1209" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1210" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1211" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1212" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1213" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1214" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1215" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1216" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1217" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1218" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1219" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1220" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1221" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1222" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1223" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1224" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1225" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1226" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1227" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1228" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1229" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1230" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1231" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1232" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1233" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1234" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1235" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1236" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1237" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1238" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1239" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1240" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1241" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1242" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1243" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1244" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1245" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1246" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1247" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1248" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1249" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1250" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1251" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>1127</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1092:A1120">
-    <sortCondition ref="A1092"/>
+  <sortState ref="C67:C165">
+    <sortCondition ref="C67:C165"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>